<commit_message>
Uzupelniona lista zdan z rekcja
</commit_message>
<xml_diff>
--- a/rektion/rektion.xlsx
+++ b/rektion/rektion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="13230" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="13236" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="537">
   <si>
     <t>ändern an D</t>
   </si>
@@ -1615,6 +1615,18 @@
   </si>
   <si>
     <t>być wściekłym na [kogoś/coś]/z powodu [kogoś/czegoś]</t>
+  </si>
+  <si>
+    <t>sich sehnen nach D</t>
+  </si>
+  <si>
+    <t>erzählen über A</t>
+  </si>
+  <si>
+    <t>kämpfen um A</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1955,19 +1967,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F271"/>
+  <dimension ref="A1:F273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="B272" sqref="B272"/>
+    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
+      <selection activeCell="A269" sqref="A269"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="2.875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="37.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="4.75" style="8" customWidth="1"/>
+    <col min="1" max="1" width="2.8984375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="37.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.69921875" style="8" customWidth="1"/>
     <col min="5" max="5" width="4.5" customWidth="1"/>
-    <col min="6" max="6" width="41.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6">
@@ -4017,7 +4029,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="257" spans="2:6">
+    <row r="257" spans="1:6">
       <c r="B257" s="8" t="s">
         <v>502</v>
       </c>
@@ -4025,7 +4037,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="258" spans="2:6">
+    <row r="258" spans="1:6">
       <c r="B258" s="8" t="s">
         <v>503</v>
       </c>
@@ -4033,7 +4045,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="259" spans="2:6">
+    <row r="259" spans="1:6">
       <c r="B259" s="8" t="s">
         <v>504</v>
       </c>
@@ -4041,7 +4053,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="260" spans="2:6">
+    <row r="260" spans="1:6">
       <c r="B260" s="8" t="s">
         <v>505</v>
       </c>
@@ -4049,7 +4061,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="261" spans="2:6">
+    <row r="261" spans="1:6">
       <c r="B261" s="8" t="s">
         <v>506</v>
       </c>
@@ -4057,7 +4069,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="262" spans="2:6">
+    <row r="262" spans="1:6">
       <c r="B262" s="8" t="s">
         <v>507</v>
       </c>
@@ -4065,7 +4077,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="263" spans="2:6">
+    <row r="263" spans="1:6">
       <c r="B263" s="8" t="s">
         <v>519</v>
       </c>
@@ -4073,7 +4085,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="264" spans="2:6">
+    <row r="264" spans="1:6">
       <c r="B264" s="8" t="s">
         <v>520</v>
       </c>
@@ -4081,7 +4093,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="265" spans="2:6">
+    <row r="265" spans="1:6">
       <c r="B265" s="8" t="s">
         <v>529</v>
       </c>
@@ -4089,7 +4101,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="266" spans="2:6">
+    <row r="266" spans="1:6">
       <c r="B266" s="8" t="s">
         <v>523</v>
       </c>
@@ -4097,7 +4109,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="267" spans="2:6">
+    <row r="267" spans="1:6">
       <c r="B267" s="8" t="s">
         <v>524</v>
       </c>
@@ -4105,23 +4117,38 @@
         <v>527</v>
       </c>
     </row>
-    <row r="268" spans="2:6">
+    <row r="268" spans="1:6">
       <c r="B268" s="8" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="269" spans="2:6">
+    <row r="269" spans="1:6">
       <c r="B269" s="8" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="270" spans="2:6">
+    <row r="270" spans="1:6">
+      <c r="A270" s="8" t="s">
+        <v>536</v>
+      </c>
       <c r="B270" s="8" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="271" spans="2:6">
-      <c r="B271" s="8"/>
+    <row r="271" spans="1:6">
+      <c r="B271" s="8" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6">
+      <c r="B272" s="8" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2">
+      <c r="B273" s="8" t="s">
+        <v>535</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4134,7 +4161,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4146,7 +4173,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Poprawki i uzupelnienia   modified:   rektion/rektion.xlsx   modified:   unr-verben/unr-verben.xlsx   modified:   wortschatz-a2/wortschatz-a2.xlsx   modified:   wortschatz-m/b-der mensch.xlsx
</commit_message>
<xml_diff>
--- a/rektion/rektion.xlsx
+++ b/rektion/rektion.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="950" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="950"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Arkusz2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Arkusz3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
+    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="544">
   <si>
     <t>ändern an D</t>
   </si>
@@ -1640,38 +1639,28 @@
   </si>
   <si>
     <t>gromadzić się w [jakimś miejscu]</t>
+  </si>
+  <si>
+    <t>sich auf-regen über A</t>
+  </si>
+  <si>
+    <t>sich mit an-geben mit D</t>
+  </si>
+  <si>
+    <t>sich an etw A machen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="4">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Czcionka tekstu podstawowego"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1683,7 +1672,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1691,2352 +1680,2596 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+  <a:themeElements>
+    <a:clrScheme name="Pakiet Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Pakiet Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Pakiet Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B1:I274"/>
+  <dimension ref="B1:I278"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="B278" sqref="B278"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.87854251012146"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.8785425101215"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="4.74898785425101"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.49797570850202"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.3765182186235"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.47773279352227"/>
+    <col min="1" max="1" width="2.8984375"/>
+    <col min="2" max="2" width="37.8984375"/>
+    <col min="3" max="4" width="4.69921875"/>
+    <col min="5" max="5" width="4.5"/>
+    <col min="6" max="6" width="41.3984375"/>
+    <col min="7" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+    <row r="1" spans="2:6">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+    <row r="2" spans="2:6">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+    <row r="4" spans="2:6">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+    <row r="5" spans="2:6">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+    <row r="9" spans="2:6">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+    <row r="10" spans="2:6">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+    <row r="11" spans="2:6">
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+    <row r="12" spans="2:6">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+    <row r="13" spans="2:6">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+    <row r="14" spans="2:6">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+    <row r="15" spans="2:6">
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+    <row r="16" spans="2:6">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+    <row r="17" spans="2:6">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+    <row r="18" spans="2:6">
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
+    <row r="19" spans="2:6">
+      <c r="B19" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
+    <row r="20" spans="2:6">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+    <row r="21" spans="2:6">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+    <row r="22" spans="2:6">
+      <c r="B22" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+    <row r="23" spans="2:6">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+    <row r="24" spans="2:6">
+      <c r="B24" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+    <row r="25" spans="2:6">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+    <row r="26" spans="2:6">
+      <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+    <row r="27" spans="2:6">
+      <c r="B27" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+    <row r="28" spans="2:6">
+      <c r="B28" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+    <row r="29" spans="2:6">
+      <c r="B29" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+    <row r="30" spans="2:6">
+      <c r="B30" t="s">
         <v>58</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+    <row r="31" spans="2:6">
+      <c r="B31" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+    <row r="32" spans="2:6">
+      <c r="B32" t="s">
         <v>62</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+    <row r="33" spans="2:6">
+      <c r="B33" t="s">
         <v>64</v>
       </c>
-      <c r="F33" s="0" t="s">
+      <c r="F33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+    <row r="34" spans="2:6">
+      <c r="B34" t="s">
         <v>66</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="F34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+    <row r="35" spans="2:6">
+      <c r="B35" t="s">
         <v>68</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="F35" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+    <row r="36" spans="2:6">
+      <c r="B36" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="F36" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+    <row r="37" spans="2:6">
+      <c r="B37" t="s">
         <v>72</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="F37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+    <row r="38" spans="2:6">
+      <c r="B38" t="s">
         <v>74</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
+    <row r="39" spans="2:6">
+      <c r="B39" t="s">
         <v>76</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="F39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
+    <row r="40" spans="2:6">
+      <c r="B40" t="s">
         <v>78</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="F40" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+    <row r="41" spans="2:6">
+      <c r="B41" t="s">
         <v>80</v>
       </c>
-      <c r="F41" s="0" t="s">
+      <c r="F41" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+    <row r="42" spans="2:6">
+      <c r="B42" t="s">
         <v>82</v>
       </c>
-      <c r="F42" s="0" t="s">
+      <c r="F42" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+    <row r="43" spans="2:6">
+      <c r="B43" t="s">
         <v>84</v>
       </c>
-      <c r="F43" s="0" t="s">
+      <c r="F43" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
+    <row r="44" spans="2:6">
+      <c r="B44" t="s">
         <v>86</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="F44" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+    <row r="45" spans="2:6">
+      <c r="B45" t="s">
         <v>88</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="F45" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+    <row r="46" spans="2:6">
+      <c r="B46" t="s">
         <v>90</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="F46" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+    <row r="47" spans="2:6">
+      <c r="B47" t="s">
         <v>92</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="F47" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="s">
+    <row r="48" spans="2:6">
+      <c r="B48" t="s">
         <v>94</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="F48" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
+    <row r="49" spans="2:6">
+      <c r="B49" t="s">
         <v>96</v>
       </c>
-      <c r="F49" s="0" t="s">
+      <c r="F49" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="0" t="s">
+    <row r="50" spans="2:6">
+      <c r="B50" t="s">
         <v>98</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="F50" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
+    <row r="51" spans="2:6">
+      <c r="B51" t="s">
         <v>100</v>
       </c>
-      <c r="F51" s="0" t="s">
+      <c r="F51" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+    <row r="52" spans="2:6">
+      <c r="B52" t="s">
         <v>102</v>
       </c>
-      <c r="F52" s="0" t="s">
+      <c r="F52" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+    <row r="53" spans="2:6">
+      <c r="B53" t="s">
         <v>104</v>
       </c>
-      <c r="F53" s="0" t="s">
+      <c r="F53" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="s">
+    <row r="54" spans="2:6">
+      <c r="B54" t="s">
         <v>106</v>
       </c>
-      <c r="F54" s="0" t="s">
+      <c r="F54" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
+    <row r="55" spans="2:6">
+      <c r="B55" t="s">
         <v>108</v>
       </c>
-      <c r="F55" s="0" t="s">
+      <c r="F55" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
+    <row r="56" spans="2:6">
+      <c r="B56" t="s">
         <v>110</v>
       </c>
-      <c r="F56" s="0" t="s">
+      <c r="F56" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
+    <row r="57" spans="2:6">
+      <c r="B57" t="s">
         <v>112</v>
       </c>
-      <c r="F57" s="0" t="s">
+      <c r="F57" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0" t="s">
+    <row r="58" spans="2:6">
+      <c r="B58" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="0" t="s">
+      <c r="F58" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0" t="s">
+    <row r="59" spans="2:6">
+      <c r="B59" t="s">
         <v>116</v>
       </c>
-      <c r="F59" s="0" t="s">
+      <c r="F59" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
+    <row r="60" spans="2:6">
+      <c r="B60" t="s">
         <v>118</v>
       </c>
-      <c r="F60" s="0" t="s">
+      <c r="F60" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="s">
+    <row r="61" spans="2:6">
+      <c r="B61" t="s">
         <v>120</v>
       </c>
-      <c r="F61" s="0" t="s">
+      <c r="F61" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
+    <row r="62" spans="2:6">
+      <c r="B62" t="s">
         <v>122</v>
       </c>
-      <c r="F62" s="0" t="s">
+      <c r="F62" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0" t="s">
+    <row r="63" spans="2:6">
+      <c r="B63" t="s">
         <v>124</v>
       </c>
-      <c r="F63" s="0" t="s">
+      <c r="F63" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="0" t="s">
+    <row r="64" spans="2:6">
+      <c r="B64" t="s">
         <v>126</v>
       </c>
-      <c r="F64" s="0" t="s">
+      <c r="F64" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="s">
+    <row r="65" spans="2:6">
+      <c r="B65" t="s">
         <v>128</v>
       </c>
-      <c r="F65" s="0" t="s">
+      <c r="F65" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="0" t="s">
+    <row r="66" spans="2:6">
+      <c r="B66" t="s">
         <v>130</v>
       </c>
-      <c r="F66" s="0" t="s">
+      <c r="F66" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0" t="s">
+    <row r="67" spans="2:6">
+      <c r="B67" t="s">
         <v>132</v>
       </c>
-      <c r="F67" s="0" t="s">
+      <c r="F67" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="0" t="s">
+    <row r="68" spans="2:6">
+      <c r="B68" t="s">
         <v>134</v>
       </c>
-      <c r="F68" s="0" t="s">
+      <c r="F68" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="0" t="s">
+    <row r="69" spans="2:6">
+      <c r="B69" t="s">
         <v>136</v>
       </c>
-      <c r="F69" s="0" t="s">
+      <c r="F69" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0" t="s">
+    <row r="70" spans="2:6">
+      <c r="B70" t="s">
         <v>138</v>
       </c>
-      <c r="F70" s="0" t="s">
+      <c r="F70" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="s">
+    <row r="71" spans="2:6">
+      <c r="B71" t="s">
         <v>140</v>
       </c>
-      <c r="F71" s="0" t="s">
+      <c r="F71" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0" t="s">
+    <row r="72" spans="2:6">
+      <c r="B72" t="s">
         <v>142</v>
       </c>
-      <c r="F72" s="0" t="s">
+      <c r="F72" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="s">
+    <row r="73" spans="2:6">
+      <c r="B73" t="s">
         <v>144</v>
       </c>
-      <c r="F73" s="0" t="s">
+      <c r="F73" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="0" t="s">
+    <row r="74" spans="2:6">
+      <c r="B74" t="s">
         <v>146</v>
       </c>
-      <c r="F74" s="0" t="s">
+      <c r="F74" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="0" t="s">
+    <row r="75" spans="2:6">
+      <c r="B75" t="s">
         <v>148</v>
       </c>
-      <c r="F75" s="0" t="s">
+      <c r="F75" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="s">
+    <row r="76" spans="2:6">
+      <c r="B76" t="s">
         <v>150</v>
       </c>
-      <c r="F76" s="0" t="s">
+      <c r="F76" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0" t="s">
+    <row r="77" spans="2:6">
+      <c r="B77" t="s">
         <v>152</v>
       </c>
-      <c r="F77" s="0" t="s">
+      <c r="F77" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0" t="s">
+    <row r="78" spans="2:6">
+      <c r="B78" t="s">
         <v>154</v>
       </c>
-      <c r="F78" s="0" t="s">
+      <c r="F78" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="0" t="s">
+    <row r="79" spans="2:6">
+      <c r="B79" t="s">
         <v>156</v>
       </c>
-      <c r="F79" s="0" t="s">
+      <c r="F79" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0" t="s">
+    <row r="80" spans="2:6">
+      <c r="B80" t="s">
         <v>158</v>
       </c>
-      <c r="F80" s="0" t="s">
+      <c r="F80" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="0" t="s">
+    <row r="81" spans="2:6">
+      <c r="B81" t="s">
         <v>160</v>
       </c>
-      <c r="F81" s="0" t="s">
+      <c r="F81" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="0" t="s">
+    <row r="82" spans="2:6">
+      <c r="B82" t="s">
         <v>162</v>
       </c>
-      <c r="F82" s="0" t="s">
+      <c r="F82" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="0" t="s">
+    <row r="83" spans="2:6">
+      <c r="B83" t="s">
         <v>164</v>
       </c>
-      <c r="F83" s="0" t="s">
+      <c r="F83" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="0" t="s">
+    <row r="84" spans="2:6">
+      <c r="B84" t="s">
         <v>166</v>
       </c>
-      <c r="F84" s="0" t="s">
+      <c r="F84" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="0" t="s">
+    <row r="85" spans="2:6" ht="15" customHeight="1">
+      <c r="B85" t="s">
         <v>168</v>
       </c>
-      <c r="F85" s="0" t="s">
+      <c r="F85" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="0" t="s">
+    <row r="86" spans="2:6">
+      <c r="B86" t="s">
         <v>170</v>
       </c>
-      <c r="F86" s="0" t="s">
+      <c r="F86" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="0" t="s">
+    <row r="87" spans="2:6">
+      <c r="B87" t="s">
         <v>172</v>
       </c>
-      <c r="F87" s="0" t="s">
+      <c r="F87" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="0" t="s">
+    <row r="88" spans="2:6">
+      <c r="B88" t="s">
         <v>174</v>
       </c>
-      <c r="F88" s="0" t="s">
+      <c r="F88" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="0" t="s">
+    <row r="89" spans="2:6">
+      <c r="B89" t="s">
         <v>176</v>
       </c>
-      <c r="F89" s="0" t="s">
+      <c r="F89" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="0" t="s">
+    <row r="90" spans="2:6">
+      <c r="B90" t="s">
         <v>178</v>
       </c>
-      <c r="F90" s="0" t="s">
+      <c r="F90" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="0" t="s">
+    <row r="91" spans="2:6">
+      <c r="B91" t="s">
         <v>180</v>
       </c>
-      <c r="F91" s="0" t="s">
+      <c r="F91" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="0" t="s">
+    <row r="92" spans="2:6">
+      <c r="B92" t="s">
         <v>182</v>
       </c>
-      <c r="F92" s="0" t="s">
+      <c r="F92" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="0" t="s">
+    <row r="93" spans="2:6">
+      <c r="B93" t="s">
         <v>184</v>
       </c>
-      <c r="F93" s="0" t="s">
+      <c r="F93" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="0" t="s">
+    <row r="94" spans="2:6">
+      <c r="B94" t="s">
         <v>186</v>
       </c>
-      <c r="F94" s="0" t="s">
+      <c r="F94" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="0" t="s">
+    <row r="95" spans="2:6">
+      <c r="B95" t="s">
         <v>188</v>
       </c>
-      <c r="F95" s="0" t="s">
+      <c r="F95" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="0" t="s">
+    <row r="96" spans="2:6">
+      <c r="B96" t="s">
         <v>190</v>
       </c>
-      <c r="F96" s="0" t="s">
+      <c r="F96" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="0" t="s">
+    <row r="97" spans="2:6">
+      <c r="B97" t="s">
         <v>192</v>
       </c>
-      <c r="F97" s="0" t="s">
+      <c r="F97" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="0" t="s">
+    <row r="98" spans="2:6">
+      <c r="B98" t="s">
         <v>194</v>
       </c>
-      <c r="F98" s="0" t="s">
+      <c r="F98" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="0" t="s">
+    <row r="99" spans="2:6">
+      <c r="B99" t="s">
         <v>196</v>
       </c>
-      <c r="F99" s="0" t="s">
+      <c r="F99" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="0" t="s">
+    <row r="100" spans="2:6">
+      <c r="B100" t="s">
         <v>198</v>
       </c>
-      <c r="F100" s="0" t="s">
+      <c r="F100" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="0" t="s">
+    <row r="101" spans="2:6">
+      <c r="B101" t="s">
         <v>200</v>
       </c>
-      <c r="F101" s="0" t="s">
+      <c r="F101" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="0" t="s">
+    <row r="102" spans="2:6">
+      <c r="B102" t="s">
         <v>202</v>
       </c>
-      <c r="F102" s="0" t="s">
+      <c r="F102" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="0" t="s">
+    <row r="103" spans="2:6">
+      <c r="B103" t="s">
         <v>204</v>
       </c>
-      <c r="F103" s="0" t="s">
+      <c r="F103" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="0" t="s">
+    <row r="104" spans="2:6">
+      <c r="B104" t="s">
         <v>206</v>
       </c>
-      <c r="F104" s="0" t="s">
+      <c r="F104" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="0" t="s">
+    <row r="105" spans="2:6">
+      <c r="B105" t="s">
         <v>208</v>
       </c>
-      <c r="F105" s="0" t="s">
+      <c r="F105" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="0" t="s">
+    <row r="106" spans="2:6">
+      <c r="B106" t="s">
         <v>210</v>
       </c>
-      <c r="F106" s="0" t="s">
+      <c r="F106" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="0" t="s">
+    <row r="107" spans="2:6">
+      <c r="B107" t="s">
         <v>212</v>
       </c>
-      <c r="F107" s="0" t="s">
+      <c r="F107" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="0" t="s">
+    <row r="108" spans="2:6">
+      <c r="B108" t="s">
         <v>214</v>
       </c>
-      <c r="F108" s="0" t="s">
+      <c r="F108" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="0" t="s">
+    <row r="109" spans="2:6">
+      <c r="B109" t="s">
         <v>216</v>
       </c>
-      <c r="F109" s="0" t="s">
+      <c r="F109" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="0" t="s">
+    <row r="110" spans="2:6">
+      <c r="B110" t="s">
         <v>218</v>
       </c>
-      <c r="F110" s="0" t="s">
+      <c r="F110" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="0" t="s">
+    <row r="111" spans="2:6">
+      <c r="B111" t="s">
         <v>220</v>
       </c>
-      <c r="F111" s="0" t="s">
+      <c r="F111" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="0" t="s">
+    <row r="112" spans="2:6">
+      <c r="B112" t="s">
         <v>222</v>
       </c>
-      <c r="F112" s="0" t="s">
+      <c r="F112" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="0" t="s">
+    <row r="113" spans="2:6">
+      <c r="B113" t="s">
         <v>224</v>
       </c>
-      <c r="F113" s="0" t="s">
+      <c r="F113" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="0" t="s">
+    <row r="114" spans="2:6">
+      <c r="B114" t="s">
         <v>226</v>
       </c>
-      <c r="F114" s="0" t="s">
+      <c r="F114" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="0" t="s">
+    <row r="115" spans="2:6">
+      <c r="B115" t="s">
         <v>226</v>
       </c>
-      <c r="F115" s="0" t="s">
+      <c r="F115" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="0" t="s">
+    <row r="116" spans="2:6">
+      <c r="B116" t="s">
         <v>229</v>
       </c>
-      <c r="F116" s="0" t="s">
+      <c r="F116" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="0" t="s">
+    <row r="117" spans="2:6">
+      <c r="B117" t="s">
         <v>231</v>
       </c>
-      <c r="F117" s="0" t="s">
+      <c r="F117" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="0" t="s">
+    <row r="118" spans="2:6">
+      <c r="B118" t="s">
         <v>233</v>
       </c>
-      <c r="F118" s="0" t="s">
+      <c r="F118" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="0" t="s">
+    <row r="119" spans="2:6">
+      <c r="B119" t="s">
         <v>235</v>
       </c>
-      <c r="F119" s="0" t="s">
+      <c r="F119" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="0" t="s">
+    <row r="120" spans="2:6">
+      <c r="B120" t="s">
         <v>237</v>
       </c>
-      <c r="F120" s="0" t="s">
+      <c r="F120" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="0" t="s">
+    <row r="121" spans="2:6">
+      <c r="B121" t="s">
         <v>239</v>
       </c>
-      <c r="F121" s="0" t="s">
+      <c r="F121" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="0" t="s">
+    <row r="122" spans="2:6">
+      <c r="B122" t="s">
         <v>241</v>
       </c>
-      <c r="F122" s="0" t="s">
+      <c r="F122" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="0" t="s">
+    <row r="123" spans="2:6">
+      <c r="B123" t="s">
         <v>243</v>
       </c>
-      <c r="F123" s="0" t="s">
+      <c r="F123" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B124" s="0" t="s">
+    <row r="124" spans="2:6">
+      <c r="B124" t="s">
         <v>245</v>
       </c>
-      <c r="F124" s="0" t="s">
+      <c r="F124" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="0" t="s">
+    <row r="125" spans="2:6">
+      <c r="B125" t="s">
         <v>247</v>
       </c>
-      <c r="F125" s="0" t="s">
+      <c r="F125" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="0" t="s">
+    <row r="126" spans="2:6">
+      <c r="B126" t="s">
         <v>249</v>
       </c>
-      <c r="F126" s="0" t="s">
+      <c r="F126" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="0" t="s">
+    <row r="127" spans="2:6">
+      <c r="B127" t="s">
         <v>251</v>
       </c>
-      <c r="F127" s="0" t="s">
+      <c r="F127" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B128" s="0" t="s">
+    <row r="128" spans="2:6">
+      <c r="B128" t="s">
         <v>253</v>
       </c>
-      <c r="F128" s="0" t="s">
+      <c r="F128" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B129" s="0" t="s">
+    <row r="129" spans="2:6">
+      <c r="B129" t="s">
         <v>255</v>
       </c>
-      <c r="F129" s="0" t="s">
+      <c r="F129" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B130" s="0" t="s">
+    <row r="130" spans="2:6">
+      <c r="B130" t="s">
         <v>257</v>
       </c>
-      <c r="F130" s="0" t="s">
+      <c r="F130" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B131" s="0" t="s">
+    <row r="131" spans="2:6">
+      <c r="B131" t="s">
         <v>259</v>
       </c>
-      <c r="F131" s="0" t="s">
+      <c r="F131" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B132" s="0" t="s">
+    <row r="132" spans="2:6">
+      <c r="B132" t="s">
         <v>261</v>
       </c>
-      <c r="F132" s="0" t="s">
+      <c r="F132" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B133" s="0" t="s">
+    <row r="133" spans="2:6">
+      <c r="B133" t="s">
         <v>263</v>
       </c>
-      <c r="F133" s="0" t="s">
+      <c r="F133" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B134" s="0" t="s">
+    <row r="134" spans="2:6">
+      <c r="B134" t="s">
         <v>265</v>
       </c>
-      <c r="F134" s="0" t="s">
+      <c r="F134" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B135" s="0" t="s">
+    <row r="135" spans="2:6">
+      <c r="B135" t="s">
         <v>267</v>
       </c>
-      <c r="F135" s="0" t="s">
+      <c r="F135" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B136" s="0" t="s">
+    <row r="136" spans="2:6">
+      <c r="B136" t="s">
         <v>269</v>
       </c>
-      <c r="F136" s="0" t="s">
+      <c r="F136" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B137" s="0" t="s">
+    <row r="137" spans="2:6">
+      <c r="B137" t="s">
         <v>271</v>
       </c>
-      <c r="F137" s="0" t="s">
+      <c r="F137" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="0" t="s">
+    <row r="138" spans="2:6">
+      <c r="B138" t="s">
         <v>273</v>
       </c>
-      <c r="F138" s="0" t="s">
+      <c r="F138" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B139" s="0" t="s">
+    <row r="139" spans="2:6">
+      <c r="B139" t="s">
         <v>275</v>
       </c>
-      <c r="F139" s="0" t="s">
+      <c r="F139" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B140" s="0" t="s">
+    <row r="140" spans="2:6">
+      <c r="B140" t="s">
         <v>277</v>
       </c>
-      <c r="F140" s="0" t="s">
+      <c r="F140" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="0" t="s">
+    <row r="141" spans="2:6">
+      <c r="B141" t="s">
         <v>279</v>
       </c>
-      <c r="F141" s="0" t="s">
+      <c r="F141" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="0" t="s">
+    <row r="142" spans="2:6">
+      <c r="B142" t="s">
         <v>281</v>
       </c>
-      <c r="F142" s="0" t="s">
+      <c r="F142" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B143" s="0" t="s">
+    <row r="143" spans="2:6">
+      <c r="B143" t="s">
         <v>283</v>
       </c>
-      <c r="F143" s="0" t="s">
+      <c r="F143" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B144" s="0" t="s">
+    <row r="144" spans="2:6">
+      <c r="B144" t="s">
         <v>285</v>
       </c>
-      <c r="F144" s="0" t="s">
+      <c r="F144" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="0" t="s">
+    <row r="145" spans="2:6">
+      <c r="B145" t="s">
         <v>287</v>
       </c>
-      <c r="F145" s="0" t="s">
+      <c r="F145" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="0" t="s">
+    <row r="146" spans="2:6">
+      <c r="B146" t="s">
         <v>289</v>
       </c>
-      <c r="F146" s="0" t="s">
+      <c r="F146" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B147" s="0" t="s">
+    <row r="147" spans="2:6">
+      <c r="B147" t="s">
         <v>291</v>
       </c>
-      <c r="F147" s="0" t="s">
+      <c r="F147" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B148" s="0" t="s">
+    <row r="148" spans="2:6">
+      <c r="B148" t="s">
         <v>293</v>
       </c>
-      <c r="F148" s="0" t="s">
+      <c r="F148" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B149" s="0" t="s">
+    <row r="149" spans="2:6">
+      <c r="B149" t="s">
         <v>295</v>
       </c>
-      <c r="F149" s="0" t="s">
+      <c r="F149" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B150" s="0" t="s">
+    <row r="150" spans="2:6">
+      <c r="B150" t="s">
         <v>297</v>
       </c>
-      <c r="F150" s="0" t="s">
+      <c r="F150" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="0" t="s">
+    <row r="151" spans="2:6">
+      <c r="B151" t="s">
         <v>299</v>
       </c>
-      <c r="F151" s="0" t="s">
+      <c r="F151" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="0" t="s">
+    <row r="152" spans="2:6">
+      <c r="B152" t="s">
         <v>301</v>
       </c>
-      <c r="F152" s="0" t="s">
+      <c r="F152" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B153" s="0" t="s">
+    <row r="153" spans="2:6">
+      <c r="B153" t="s">
         <v>303</v>
       </c>
-      <c r="F153" s="0" t="s">
+      <c r="F153" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B154" s="0" t="s">
+    <row r="154" spans="2:6">
+      <c r="B154" t="s">
         <v>305</v>
       </c>
-      <c r="F154" s="0" t="s">
+      <c r="F154" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B155" s="0" t="s">
+    <row r="155" spans="2:6">
+      <c r="B155" t="s">
         <v>307</v>
       </c>
-      <c r="F155" s="0" t="s">
+      <c r="F155" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B156" s="0" t="s">
+    <row r="156" spans="2:6">
+      <c r="B156" t="s">
         <v>309</v>
       </c>
-      <c r="F156" s="0" t="s">
+      <c r="F156" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B157" s="0" t="s">
+    <row r="157" spans="2:6">
+      <c r="B157" t="s">
         <v>311</v>
       </c>
-      <c r="F157" s="0" t="s">
+      <c r="F157" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B158" s="0" t="s">
+    <row r="158" spans="2:6">
+      <c r="B158" t="s">
         <v>313</v>
       </c>
-      <c r="F158" s="0" t="s">
+      <c r="F158" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B159" s="0" t="s">
+    <row r="159" spans="2:6">
+      <c r="B159" t="s">
         <v>315</v>
       </c>
-      <c r="F159" s="0" t="s">
+      <c r="F159" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B160" s="0" t="s">
+    <row r="160" spans="2:6">
+      <c r="B160" t="s">
         <v>317</v>
       </c>
-      <c r="F160" s="0" t="s">
+      <c r="F160" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B161" s="0" t="s">
+    <row r="161" spans="2:6">
+      <c r="B161" t="s">
         <v>319</v>
       </c>
-      <c r="F161" s="0" t="s">
+      <c r="F161" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B162" s="0" t="s">
+    <row r="162" spans="2:6">
+      <c r="B162" t="s">
         <v>321</v>
       </c>
-      <c r="F162" s="0" t="s">
+      <c r="F162" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B163" s="0" t="s">
+    <row r="163" spans="2:6">
+      <c r="B163" t="s">
         <v>323</v>
       </c>
-      <c r="F163" s="0" t="s">
+      <c r="F163" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B164" s="0" t="s">
+    <row r="164" spans="2:6">
+      <c r="B164" t="s">
         <v>325</v>
       </c>
-      <c r="F164" s="0" t="s">
+      <c r="F164" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B165" s="0" t="s">
+    <row r="165" spans="2:6">
+      <c r="B165" t="s">
         <v>327</v>
       </c>
-      <c r="F165" s="0" t="s">
+      <c r="F165" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B166" s="0" t="s">
+    <row r="166" spans="2:6">
+      <c r="B166" t="s">
         <v>329</v>
       </c>
-      <c r="F166" s="0" t="s">
+      <c r="F166" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B167" s="0" t="s">
+    <row r="167" spans="2:6">
+      <c r="B167" t="s">
         <v>331</v>
       </c>
-      <c r="F167" s="0" t="s">
+      <c r="F167" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B168" s="0" t="s">
+    <row r="168" spans="2:6">
+      <c r="B168" t="s">
         <v>333</v>
       </c>
-      <c r="F168" s="0" t="s">
+      <c r="F168" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B169" s="0" t="s">
+    <row r="169" spans="2:6">
+      <c r="B169" t="s">
         <v>335</v>
       </c>
-      <c r="F169" s="0" t="s">
+      <c r="F169" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B170" s="0" t="s">
+    <row r="170" spans="2:6">
+      <c r="B170" t="s">
         <v>337</v>
       </c>
-      <c r="F170" s="0" t="s">
+      <c r="F170" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B171" s="0" t="s">
+    <row r="171" spans="2:6">
+      <c r="B171" t="s">
         <v>339</v>
       </c>
-      <c r="F171" s="0" t="s">
+      <c r="F171" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B172" s="0" t="s">
+    <row r="172" spans="2:6">
+      <c r="B172" t="s">
         <v>341</v>
       </c>
-      <c r="F172" s="0" t="s">
+      <c r="F172" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B173" s="0" t="s">
+    <row r="173" spans="2:6">
+      <c r="B173" t="s">
         <v>343</v>
       </c>
-      <c r="F173" s="0" t="s">
+      <c r="F173" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B174" s="0" t="s">
+    <row r="174" spans="2:6">
+      <c r="B174" t="s">
         <v>345</v>
       </c>
-      <c r="F174" s="0" t="s">
+      <c r="F174" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B175" s="0" t="s">
+    <row r="175" spans="2:6">
+      <c r="B175" t="s">
         <v>347</v>
       </c>
-      <c r="F175" s="0" t="s">
+      <c r="F175" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B176" s="0" t="s">
+    <row r="176" spans="2:6">
+      <c r="B176" t="s">
         <v>349</v>
       </c>
-      <c r="F176" s="0" t="s">
+      <c r="F176" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B177" s="0" t="s">
+    <row r="177" spans="2:6">
+      <c r="B177" t="s">
         <v>351</v>
       </c>
-      <c r="F177" s="0" t="s">
+      <c r="F177" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B178" s="0" t="s">
+    <row r="178" spans="2:6">
+      <c r="B178" t="s">
         <v>353</v>
       </c>
-      <c r="F178" s="0" t="s">
+      <c r="F178" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B179" s="0" t="s">
+    <row r="179" spans="2:6">
+      <c r="B179" t="s">
         <v>355</v>
       </c>
-      <c r="F179" s="0" t="s">
+      <c r="F179" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B180" s="0" t="s">
+    <row r="180" spans="2:6">
+      <c r="B180" t="s">
         <v>357</v>
       </c>
-      <c r="F180" s="0" t="s">
+      <c r="F180" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B181" s="0" t="s">
+    <row r="181" spans="2:6">
+      <c r="B181" t="s">
         <v>359</v>
       </c>
-      <c r="F181" s="0" t="s">
+      <c r="F181" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B182" s="0" t="s">
+    <row r="182" spans="2:6">
+      <c r="B182" t="s">
         <v>361</v>
       </c>
-      <c r="F182" s="0" t="s">
+      <c r="F182" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B183" s="0" t="s">
+    <row r="183" spans="2:6">
+      <c r="B183" t="s">
         <v>363</v>
       </c>
-      <c r="F183" s="0" t="s">
+      <c r="F183" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B184" s="0" t="s">
+    <row r="184" spans="2:6">
+      <c r="B184" t="s">
         <v>365</v>
       </c>
-      <c r="F184" s="0" t="s">
+      <c r="F184" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B185" s="0" t="s">
+    <row r="185" spans="2:6">
+      <c r="B185" t="s">
         <v>367</v>
       </c>
-      <c r="F185" s="0" t="s">
+      <c r="F185" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B186" s="0" t="s">
+    <row r="186" spans="2:6">
+      <c r="B186" t="s">
         <v>369</v>
       </c>
-      <c r="F186" s="0" t="s">
+      <c r="F186" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B187" s="0" t="s">
+    <row r="187" spans="2:6">
+      <c r="B187" t="s">
         <v>371</v>
       </c>
-      <c r="F187" s="0" t="s">
+      <c r="F187" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B188" s="0" t="s">
+    <row r="188" spans="2:6">
+      <c r="B188" t="s">
         <v>373</v>
       </c>
-      <c r="F188" s="0" t="s">
+      <c r="F188" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B189" s="0" t="s">
+    <row r="189" spans="2:6">
+      <c r="B189" t="s">
         <v>375</v>
       </c>
-      <c r="F189" s="0" t="s">
+      <c r="F189" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B190" s="0" t="s">
+    <row r="190" spans="2:6">
+      <c r="B190" t="s">
         <v>377</v>
       </c>
-      <c r="F190" s="0" t="s">
+      <c r="F190" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B191" s="0" t="s">
+    <row r="191" spans="2:6">
+      <c r="B191" t="s">
         <v>379</v>
       </c>
-      <c r="F191" s="0" t="s">
+      <c r="F191" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B192" s="0" t="s">
+    <row r="192" spans="2:6">
+      <c r="B192" t="s">
         <v>381</v>
       </c>
-      <c r="F192" s="0" t="s">
+      <c r="F192" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B193" s="0" t="s">
+    <row r="193" spans="2:6">
+      <c r="B193" t="s">
         <v>383</v>
       </c>
-      <c r="F193" s="0" t="s">
+      <c r="F193" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B194" s="0" t="s">
+    <row r="194" spans="2:6">
+      <c r="B194" t="s">
         <v>385</v>
       </c>
-      <c r="F194" s="0" t="s">
+      <c r="F194" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B195" s="0" t="s">
+    <row r="195" spans="2:6">
+      <c r="B195" t="s">
         <v>387</v>
       </c>
-      <c r="F195" s="0" t="s">
+      <c r="F195" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B196" s="0" t="s">
+    <row r="196" spans="2:6">
+      <c r="B196" t="s">
         <v>389</v>
       </c>
-      <c r="F196" s="0" t="s">
+      <c r="F196" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B197" s="0" t="s">
+    <row r="197" spans="2:6">
+      <c r="B197" t="s">
         <v>391</v>
       </c>
-      <c r="F197" s="0" t="s">
+      <c r="F197" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B198" s="0" t="s">
+    <row r="198" spans="2:6">
+      <c r="B198" t="s">
         <v>393</v>
       </c>
-      <c r="F198" s="0" t="s">
+      <c r="F198" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B199" s="0" t="s">
+    <row r="199" spans="2:6">
+      <c r="B199" t="s">
         <v>395</v>
       </c>
-      <c r="F199" s="0" t="s">
+      <c r="F199" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B200" s="0" t="s">
+    <row r="200" spans="2:6">
+      <c r="B200" t="s">
         <v>397</v>
       </c>
-      <c r="F200" s="0" t="s">
+      <c r="F200" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B201" s="0" t="s">
+    <row r="201" spans="2:6">
+      <c r="B201" t="s">
         <v>399</v>
       </c>
-      <c r="F201" s="0" t="s">
+      <c r="F201" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B202" s="0" t="s">
+    <row r="202" spans="2:6">
+      <c r="B202" t="s">
         <v>401</v>
       </c>
       <c r="E202" s="1"/>
-      <c r="F202" s="0" t="s">
+      <c r="F202" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B203" s="0" t="s">
+    <row r="203" spans="2:6">
+      <c r="B203" t="s">
         <v>403</v>
       </c>
       <c r="E203" s="1"/>
-      <c r="F203" s="0" t="s">
+      <c r="F203" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B204" s="0" t="s">
+    <row r="204" spans="2:6">
+      <c r="B204" t="s">
         <v>405</v>
       </c>
       <c r="E204" s="1"/>
-      <c r="F204" s="0" t="s">
+      <c r="F204" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B205" s="0" t="s">
+    <row r="205" spans="2:6">
+      <c r="B205" t="s">
         <v>407</v>
       </c>
       <c r="E205" s="1"/>
-      <c r="F205" s="0" t="s">
+      <c r="F205" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B206" s="0" t="s">
+    <row r="206" spans="2:6">
+      <c r="B206" t="s">
         <v>409</v>
       </c>
       <c r="E206" s="1"/>
-      <c r="F206" s="0" t="s">
+      <c r="F206" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B207" s="0" t="s">
+    <row r="207" spans="2:6">
+      <c r="B207" t="s">
         <v>411</v>
       </c>
       <c r="E207" s="1"/>
-      <c r="F207" s="0" t="s">
+      <c r="F207" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B208" s="0" t="s">
+    <row r="208" spans="2:6">
+      <c r="B208" t="s">
         <v>413</v>
       </c>
-      <c r="F208" s="0" t="s">
+      <c r="F208" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B209" s="0" t="s">
+    <row r="209" spans="2:6">
+      <c r="B209" t="s">
         <v>415</v>
       </c>
-      <c r="F209" s="0" t="s">
+      <c r="F209" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B210" s="0" t="s">
+    <row r="210" spans="2:6">
+      <c r="B210" t="s">
         <v>417</v>
       </c>
-      <c r="F210" s="0" t="s">
+      <c r="F210" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B211" s="0" t="s">
+    <row r="211" spans="2:6">
+      <c r="B211" t="s">
         <v>419</v>
       </c>
-      <c r="F211" s="0" t="s">
+      <c r="F211" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B212" s="0" t="s">
+    <row r="212" spans="2:6">
+      <c r="B212" t="s">
         <v>421</v>
       </c>
-      <c r="F212" s="0" t="s">
+      <c r="F212" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B213" s="0" t="s">
+    <row r="213" spans="2:6">
+      <c r="B213" t="s">
         <v>423</v>
       </c>
-      <c r="F213" s="0" t="s">
+      <c r="F213" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B214" s="0" t="s">
+    <row r="214" spans="2:6">
+      <c r="B214" t="s">
         <v>425</v>
       </c>
-      <c r="F214" s="0" t="s">
+      <c r="F214" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B215" s="0" t="s">
+    <row r="215" spans="2:6">
+      <c r="B215" t="s">
         <v>427</v>
       </c>
-      <c r="F215" s="0" t="s">
+      <c r="F215" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B216" s="0" t="s">
+    <row r="216" spans="2:6">
+      <c r="B216" t="s">
         <v>429</v>
       </c>
-      <c r="F216" s="0" t="s">
+      <c r="F216" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B217" s="0" t="s">
+    <row r="217" spans="2:6">
+      <c r="B217" t="s">
         <v>431</v>
       </c>
-      <c r="F217" s="0" t="s">
+      <c r="F217" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B218" s="0" t="s">
+    <row r="218" spans="2:6">
+      <c r="B218" t="s">
         <v>433</v>
       </c>
-      <c r="F218" s="0" t="s">
+      <c r="F218" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B219" s="0" t="s">
+    <row r="219" spans="2:6">
+      <c r="B219" t="s">
         <v>435</v>
       </c>
-      <c r="F219" s="0" t="s">
+      <c r="F219" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B220" s="0" t="s">
+    <row r="220" spans="2:6">
+      <c r="B220" t="s">
         <v>437</v>
       </c>
-      <c r="F220" s="0" t="s">
+      <c r="F220" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B221" s="0" t="s">
+    <row r="221" spans="2:6">
+      <c r="B221" t="s">
         <v>439</v>
       </c>
-      <c r="F221" s="0" t="s">
+      <c r="F221" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B222" s="0" t="s">
+    <row r="222" spans="2:6">
+      <c r="B222" t="s">
         <v>441</v>
       </c>
-      <c r="F222" s="0" t="s">
+      <c r="F222" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B223" s="0" t="s">
+    <row r="223" spans="2:6">
+      <c r="B223" t="s">
         <v>443</v>
       </c>
-      <c r="F223" s="0" t="s">
+      <c r="F223" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B224" s="0" t="s">
+    <row r="224" spans="2:6">
+      <c r="B224" t="s">
         <v>445</v>
       </c>
-      <c r="F224" s="0" t="s">
+      <c r="F224" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B225" s="0" t="s">
+    <row r="225" spans="2:6">
+      <c r="B225" t="s">
         <v>447</v>
       </c>
-      <c r="F225" s="0" t="s">
+      <c r="F225" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B226" s="0" t="s">
+    <row r="226" spans="2:6">
+      <c r="B226" t="s">
         <v>449</v>
       </c>
-      <c r="F226" s="0" t="s">
+      <c r="F226" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B227" s="0" t="s">
+    <row r="227" spans="2:6">
+      <c r="B227" t="s">
         <v>451</v>
       </c>
-      <c r="F227" s="0" t="s">
+      <c r="F227" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B228" s="0" t="s">
+    <row r="228" spans="2:6">
+      <c r="B228" t="s">
         <v>453</v>
       </c>
-      <c r="F228" s="0" t="s">
+      <c r="F228" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B229" s="0" t="s">
+    <row r="229" spans="2:6">
+      <c r="B229" t="s">
         <v>455</v>
       </c>
-      <c r="F229" s="0" t="s">
+      <c r="F229" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B230" s="0" t="s">
+    <row r="230" spans="2:6">
+      <c r="B230" t="s">
         <v>457</v>
       </c>
-      <c r="F230" s="0" t="s">
+      <c r="F230" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B231" s="0" t="s">
+    <row r="231" spans="2:6">
+      <c r="B231" t="s">
         <v>459</v>
       </c>
-      <c r="F231" s="0" t="s">
+      <c r="F231" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B232" s="0" t="s">
+    <row r="232" spans="2:6">
+      <c r="B232" t="s">
         <v>461</v>
       </c>
-      <c r="F232" s="0" t="s">
+      <c r="F232" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B233" s="0" t="s">
+    <row r="233" spans="2:6">
+      <c r="B233" t="s">
         <v>463</v>
       </c>
-      <c r="F233" s="0" t="s">
+      <c r="F233" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B234" s="0" t="s">
+    <row r="234" spans="2:6">
+      <c r="B234" t="s">
         <v>465</v>
       </c>
-      <c r="F234" s="0" t="s">
+      <c r="F234" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B235" s="0" t="s">
+    <row r="235" spans="2:6">
+      <c r="B235" t="s">
         <v>467</v>
       </c>
-      <c r="F235" s="0" t="s">
+      <c r="F235" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B236" s="0" t="s">
+    <row r="236" spans="2:6">
+      <c r="B236" t="s">
         <v>469</v>
       </c>
-      <c r="F236" s="0" t="s">
+      <c r="F236" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B237" s="0" t="s">
+    <row r="237" spans="2:6">
+      <c r="B237" t="s">
         <v>471</v>
       </c>
-      <c r="F237" s="0" t="s">
+      <c r="F237" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B238" s="0" t="s">
+    <row r="238" spans="2:6">
+      <c r="B238" t="s">
         <v>473</v>
       </c>
-      <c r="F238" s="0" t="s">
+      <c r="F238" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B239" s="0" t="s">
+    <row r="239" spans="2:6">
+      <c r="B239" t="s">
         <v>475</v>
       </c>
-      <c r="F239" s="0" t="s">
+      <c r="F239" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B240" s="0" t="s">
+    <row r="240" spans="2:6">
+      <c r="B240" t="s">
         <v>477</v>
       </c>
-      <c r="F240" s="0" t="s">
+      <c r="F240" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B241" s="0" t="s">
+    <row r="241" spans="2:6">
+      <c r="B241" t="s">
         <v>479</v>
       </c>
-      <c r="F241" s="0" t="s">
+      <c r="F241" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B242" s="0" t="s">
+    <row r="242" spans="2:6">
+      <c r="B242" t="s">
         <v>481</v>
       </c>
-      <c r="F242" s="0" t="s">
+      <c r="F242" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B243" s="0" t="s">
+    <row r="243" spans="2:6">
+      <c r="B243" t="s">
         <v>483</v>
       </c>
-      <c r="F243" s="0" t="s">
+      <c r="F243" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B245" s="0" t="s">
+    <row r="245" spans="2:6">
+      <c r="B245" t="s">
         <v>485</v>
       </c>
-      <c r="F245" s="0" t="s">
+      <c r="F245" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B246" s="0" t="s">
+    <row r="246" spans="2:6">
+      <c r="B246" t="s">
         <v>487</v>
       </c>
-      <c r="F246" s="0" t="s">
+      <c r="F246" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B247" s="0" t="s">
+    <row r="247" spans="2:6">
+      <c r="B247" t="s">
         <v>489</v>
       </c>
-      <c r="F247" s="0" t="s">
+      <c r="F247" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B248" s="0" t="s">
+    <row r="248" spans="2:6">
+      <c r="B248" t="s">
         <v>491</v>
       </c>
-      <c r="F248" s="0" t="s">
+      <c r="F248" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B249" s="0" t="s">
+    <row r="249" spans="2:6">
+      <c r="B249" t="s">
         <v>493</v>
       </c>
-      <c r="F249" s="0" t="s">
+      <c r="F249" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B250" s="0" t="s">
+    <row r="250" spans="2:6">
+      <c r="B250" t="s">
         <v>495</v>
       </c>
-      <c r="F250" s="0" t="s">
+      <c r="F250" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B251" s="0" t="s">
+    <row r="251" spans="2:6">
+      <c r="B251" t="s">
         <v>497</v>
       </c>
-      <c r="F251" s="0" t="s">
+      <c r="F251" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B252" s="0" t="s">
+    <row r="252" spans="2:6">
+      <c r="B252" t="s">
         <v>499</v>
       </c>
-      <c r="F252" s="0" t="s">
+      <c r="F252" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B253" s="0" t="s">
+    <row r="253" spans="2:6">
+      <c r="B253" t="s">
         <v>501</v>
       </c>
-      <c r="F253" s="0" t="s">
+      <c r="F253" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B254" s="0" t="s">
+    <row r="254" spans="2:6">
+      <c r="B254" t="s">
         <v>503</v>
       </c>
-      <c r="F254" s="0" t="s">
+      <c r="F254" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B255" s="0" t="s">
+    <row r="255" spans="2:6">
+      <c r="B255" t="s">
         <v>505</v>
       </c>
-      <c r="F255" s="0" t="s">
+      <c r="F255" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B256" s="0" t="s">
+    <row r="256" spans="2:6">
+      <c r="B256" t="s">
         <v>507</v>
       </c>
-      <c r="F256" s="0" t="s">
+      <c r="F256" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B257" s="0" t="s">
+    <row r="257" spans="2:9">
+      <c r="B257" t="s">
         <v>509</v>
       </c>
-      <c r="F257" s="0" t="s">
+      <c r="F257" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B258" s="0" t="s">
+    <row r="258" spans="2:9">
+      <c r="B258" t="s">
         <v>511</v>
       </c>
-      <c r="F258" s="0" t="s">
+      <c r="F258" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B259" s="0" t="s">
+    <row r="259" spans="2:9">
+      <c r="B259" t="s">
         <v>513</v>
       </c>
-      <c r="F259" s="0" t="s">
+      <c r="F259" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B260" s="0" t="s">
+    <row r="260" spans="2:9">
+      <c r="B260" t="s">
         <v>515</v>
       </c>
-      <c r="F260" s="0" t="s">
+      <c r="F260" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B261" s="0" t="s">
+    <row r="261" spans="2:9">
+      <c r="B261" t="s">
         <v>517</v>
       </c>
-      <c r="F261" s="0" t="s">
+      <c r="F261" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B262" s="0" t="s">
+    <row r="262" spans="2:9">
+      <c r="B262" t="s">
         <v>519</v>
       </c>
-      <c r="F262" s="0" t="s">
+      <c r="F262" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B263" s="0" t="s">
+    <row r="263" spans="2:9">
+      <c r="B263" t="s">
         <v>521</v>
       </c>
-      <c r="F263" s="0" t="s">
+      <c r="F263" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B264" s="0" t="s">
+    <row r="264" spans="2:9">
+      <c r="B264" t="s">
         <v>523</v>
       </c>
-      <c r="F264" s="0" t="s">
+      <c r="F264" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B265" s="0" t="s">
+    <row r="265" spans="2:9">
+      <c r="B265" t="s">
         <v>525</v>
       </c>
-      <c r="F265" s="0" t="s">
+      <c r="F265" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B266" s="0" t="s">
+    <row r="266" spans="2:9">
+      <c r="B266" t="s">
         <v>527</v>
       </c>
-      <c r="F266" s="0" t="s">
+      <c r="F266" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B267" s="0" t="s">
+    <row r="267" spans="2:9">
+      <c r="B267" t="s">
         <v>529</v>
       </c>
-      <c r="F267" s="0" t="s">
+      <c r="F267" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B268" s="0" t="s">
+    <row r="268" spans="2:9">
+      <c r="B268" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B269" s="0" t="s">
+    <row r="269" spans="2:9">
+      <c r="B269" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B270" s="0" t="s">
+    <row r="270" spans="2:9">
+      <c r="B270" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B271" s="0" t="s">
+    <row r="271" spans="2:9">
+      <c r="B271" t="s">
         <v>533</v>
       </c>
-      <c r="F271" s="0" t="s">
+      <c r="F271" t="s">
         <v>534</v>
       </c>
       <c r="G271" s="2" t="str">
-        <f aca="false">IF(AND(EXACT(MID(B271,1,1),UPPER(MID(B271,1,1))),NOT(OR(ISNUMBER(FIND(".",B271,1)),ISNUMBER(FIND("?",B271,1)),ISNUMBER(FIND("!",B271,1)))),COUNTA(C271)&gt;0), "(+ Pl.)", IF(EXACT(MID(B271,LEN(B271)-1,2),"en"), CONCATENATE(IF(OR(COUNTA(C271)&gt;0,COUNTA(D271)&gt;0,COUNTA(E271)&gt;0),"(+ ",""),IF(COUNTA(C271)&gt;0,"Präsens",""),IF(AND(COUNTA(C271)&gt;0,OR(COUNTA(D271)&gt;0,COUNTA(E271)&gt;0)),", ",""),IF(COUNTA(D271)&gt;0,"Imperfekt",""),IF(AND(OR(COUNTA(C271)&gt;0,COUNTA(D271)&gt;0),COUNTA(E271)&gt;0),", ",""),IF(COUNTA(E271)&gt;0,"P. II",""),IF(OR(COUNTA(C271)&gt;0,COUNTA(D271)&gt;0,COUNTA(E271)&gt;0),")","")), ""))</f>
+        <f t="shared" ref="G271:G276" si="0">IF(AND(EXACT(MID(B271,1,1),UPPER(MID(B271,1,1))),NOT(OR(ISNUMBER(FIND(".",B271,1)),ISNUMBER(FIND("?",B271,1)),ISNUMBER(FIND("!",B271,1)))),COUNTA(C271)&gt;0), "(+ Pl.)", IF(EXACT(MID(B271,LEN(B271)-1,2),"en"), CONCATENATE(IF(OR(COUNTA(C271)&gt;0,COUNTA(D271)&gt;0,COUNTA(E271)&gt;0),"(+ ",""),IF(COUNTA(C271)&gt;0,"Präsens",""),IF(AND(COUNTA(C271)&gt;0,OR(COUNTA(D271)&gt;0,COUNTA(E271)&gt;0)),", ",""),IF(COUNTA(D271)&gt;0,"Imperfekt",""),IF(AND(OR(COUNTA(C271)&gt;0,COUNTA(D271)&gt;0),COUNTA(E271)&gt;0),", ",""),IF(COUNTA(E271)&gt;0,"P. II",""),IF(OR(COUNTA(C271)&gt;0,COUNTA(D271)&gt;0,COUNTA(E271)&gt;0),")","")), ""))</f>
         <v/>
       </c>
-      <c r="H271" s="0" t="n">
+      <c r="H271">
         <v>107</v>
       </c>
-      <c r="I271" s="0" t="n">
+      <c r="I271">
         <v>1404</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B272" s="0" t="s">
+    <row r="272" spans="2:9">
+      <c r="B272" t="s">
         <v>535</v>
       </c>
-      <c r="F272" s="0" t="s">
+      <c r="F272" t="s">
         <v>536</v>
       </c>
       <c r="G272" s="2" t="str">
-        <f aca="false">IF(AND(EXACT(MID(B272,1,1),UPPER(MID(B272,1,1))),NOT(OR(ISNUMBER(FIND(".",B272,1)),ISNUMBER(FIND("?",B272,1)),ISNUMBER(FIND("!",B272,1)))),COUNTA(C272)&gt;0), "(+ Pl.)", IF(EXACT(MID(B272,LEN(B272)-1,2),"en"), CONCATENATE(IF(OR(COUNTA(C272)&gt;0,COUNTA(D272)&gt;0,COUNTA(E272)&gt;0),"(+ ",""),IF(COUNTA(C272)&gt;0,"Präsens",""),IF(AND(COUNTA(C272)&gt;0,OR(COUNTA(D272)&gt;0,COUNTA(E272)&gt;0)),", ",""),IF(COUNTA(D272)&gt;0,"Imperfekt",""),IF(AND(OR(COUNTA(C272)&gt;0,COUNTA(D272)&gt;0),COUNTA(E272)&gt;0),", ",""),IF(COUNTA(E272)&gt;0,"P. II",""),IF(OR(COUNTA(C272)&gt;0,COUNTA(D272)&gt;0,COUNTA(E272)&gt;0),")","")), ""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H272" s="0" t="n">
+      <c r="H272">
         <v>104</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B273" s="0" t="s">
+    <row r="273" spans="2:9">
+      <c r="B273" t="s">
         <v>537</v>
       </c>
-      <c r="F273" s="0" t="s">
+      <c r="F273" t="s">
         <v>538</v>
       </c>
       <c r="G273" s="2" t="str">
-        <f aca="false">IF(AND(EXACT(MID(B273,1,1),UPPER(MID(B273,1,1))),NOT(OR(ISNUMBER(FIND(".",B273,1)),ISNUMBER(FIND("?",B273,1)),ISNUMBER(FIND("!",B273,1)))),COUNTA(C273)&gt;0), "(+ Pl.)", IF(EXACT(MID(B273,LEN(B273)-1,2),"en"), CONCATENATE(IF(OR(COUNTA(C273)&gt;0,COUNTA(D273)&gt;0,COUNTA(E273)&gt;0),"(+ ",""),IF(COUNTA(C273)&gt;0,"Präsens",""),IF(AND(COUNTA(C273)&gt;0,OR(COUNTA(D273)&gt;0,COUNTA(E273)&gt;0)),", ",""),IF(COUNTA(D273)&gt;0,"Imperfekt",""),IF(AND(OR(COUNTA(C273)&gt;0,COUNTA(D273)&gt;0),COUNTA(E273)&gt;0),", ",""),IF(COUNTA(E273)&gt;0,"P. II",""),IF(OR(COUNTA(C273)&gt;0,COUNTA(D273)&gt;0,COUNTA(E273)&gt;0),")","")), ""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H273" s="0" t="n">
+      <c r="H273">
         <v>105</v>
       </c>
-      <c r="I273" s="0" t="n">
+      <c r="I273">
         <v>106</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B274" s="0" t="s">
+    <row r="274" spans="2:9">
+      <c r="B274" t="s">
         <v>539</v>
       </c>
       <c r="C274" s="1"/>
-      <c r="F274" s="0" t="s">
+      <c r="F274" t="s">
         <v>540</v>
       </c>
       <c r="G274" s="2" t="str">
-        <f aca="false">IF(AND(EXACT(MID(B274,1,1),UPPER(MID(B274,1,1))),NOT(OR(ISNUMBER(FIND(".",B274,1)),ISNUMBER(FIND("?",B274,1)),ISNUMBER(FIND("!",B274,1)))),COUNTA(C274)&gt;0), "(+ Pl.)", IF(EXACT(MID(B274,LEN(B274)-1,2),"en"), CONCATENATE(IF(OR(COUNTA(C274)&gt;0,COUNTA(D274)&gt;0,COUNTA(E274)&gt;0),"(+ ",""),IF(COUNTA(C274)&gt;0,"Präsens",""),IF(AND(COUNTA(C274)&gt;0,OR(COUNTA(D274)&gt;0,COUNTA(E274)&gt;0)),", ",""),IF(COUNTA(D274)&gt;0,"Imperfekt",""),IF(AND(OR(COUNTA(C274)&gt;0,COUNTA(D274)&gt;0),COUNTA(E274)&gt;0),", ",""),IF(COUNTA(E274)&gt;0,"P. II",""),IF(OR(COUNTA(C274)&gt;0,COUNTA(D274)&gt;0,COUNTA(E274)&gt;0),")","")), ""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H274" s="0" t="n">
+      <c r="H274">
         <v>1700</v>
       </c>
     </row>
+    <row r="275" spans="2:9">
+      <c r="B275" t="s">
+        <v>541</v>
+      </c>
+      <c r="G275" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="276" spans="2:9">
+      <c r="B276" t="s">
+        <v>542</v>
+      </c>
+      <c r="G276" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="278" spans="2:9">
+      <c r="B278" t="s">
+        <v>543</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.47773279352227"/>
+    <col min="1" max="1025" width="8.5"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.47773279352227"/>
+    <col min="1" max="1025" width="8.5"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>